<commit_message>
add new exels to import in DataBase
</commit_message>
<xml_diff>
--- a/backend/exels/components-count.xlsx
+++ b/backend/exels/components-count.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Александр\Desktop\sklad\exel-file\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Александр\Desktop\Portfolio\React-projects\crm\backend\exels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B79D3D0-6591-4D51-9861-D4E6A33FAFB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BE4D32-E805-4ABD-9501-15DA0DD6B110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="202">
   <si>
     <t xml:space="preserve">Амортизаторы </t>
   </si>
@@ -457,19 +457,198 @@
   </si>
   <si>
     <t>Мироновская</t>
+  </si>
+  <si>
+    <t>Вакуумный пакет 25х30 см, ПЭТ/ПЭ, 62 мкм</t>
+  </si>
+  <si>
+    <t>Зип блест. 12x18 см</t>
+  </si>
+  <si>
+    <t>Зип блест. 16х22 см</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Зип блест. 20,5х26 </t>
+  </si>
+  <si>
+    <t>Зип блест. 7х8 см</t>
+  </si>
+  <si>
+    <t>Зип блест. 9x10 см</t>
+  </si>
+  <si>
+    <t>Зип прозрачный 10х15 см</t>
+  </si>
+  <si>
+    <t>Зип прозрачный 10х30 см</t>
+  </si>
+  <si>
+    <t>Зип прозрачный 15х20 см</t>
+  </si>
+  <si>
+    <t>Зип прозрачный 15х22 см</t>
+  </si>
+  <si>
+    <t>Зип прозрачный 15х30 см</t>
+  </si>
+  <si>
+    <t>Зип прозрачный 15х40 см</t>
+  </si>
+  <si>
+    <t>Зип прозрачный 18х25 см</t>
+  </si>
+  <si>
+    <t>Зип прозрачный 20х30 см</t>
+  </si>
+  <si>
+    <t>Зип прозрачный 6х6 (винт носоупор)</t>
+  </si>
+  <si>
+    <t>Коробка для очков 20х10х5</t>
+  </si>
+  <si>
+    <t>Пакет блест. 20,5х26 без зип</t>
+  </si>
+  <si>
+    <t>Пакет блест. 40х32 см без зип</t>
+  </si>
+  <si>
+    <t>Пакет БОПП с клеевым клапаном 15х20 см</t>
+  </si>
+  <si>
+    <t>Пакет ПВД 35х40 см (мячи)</t>
+  </si>
+  <si>
+    <t>Набор для очков 3 шт</t>
+  </si>
+  <si>
+    <t>Набор для очков 6 шт</t>
+  </si>
+  <si>
+    <t>Сверло ступенчатое набор 3 шт без кернера</t>
+  </si>
+  <si>
+    <t>Сверло ступенчатое набор 3 шт с кернером</t>
+  </si>
+  <si>
+    <t>Сверло ступенчатое набор 6 шт без кернера</t>
+  </si>
+  <si>
+    <t>Сверло ступенчатое набор 7 шт в кейсе</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сверло ступенчатое набор мини 3 шт без кернера </t>
+  </si>
+  <si>
+    <t>Сверло-метчик набор 6 шт</t>
+  </si>
+  <si>
+    <t>CARRERA_5046/S</t>
+  </si>
+  <si>
+    <t>P8317</t>
+  </si>
+  <si>
+    <t>P8317_0BM</t>
+  </si>
+  <si>
+    <t>PLD _1016/S/NEW</t>
+  </si>
+  <si>
+    <t>PLD_2053/S</t>
+  </si>
+  <si>
+    <t>PLD_2088/S</t>
+  </si>
+  <si>
+    <t>PLD_2098/S</t>
+  </si>
+  <si>
+    <t>PLD_2119/G/S</t>
+  </si>
+  <si>
+    <t>PLD_2121/S</t>
+  </si>
+  <si>
+    <t>PLD_2123/S_D51</t>
+  </si>
+  <si>
+    <t>PLD_2123BlackGrey</t>
+  </si>
+  <si>
+    <t>PLD_2138/S</t>
+  </si>
+  <si>
+    <t>PLD_2138/S_O6W</t>
+  </si>
+  <si>
+    <t>PLD_2139/S</t>
+  </si>
+  <si>
+    <t>PLD_2149/S</t>
+  </si>
+  <si>
+    <t>PLD_3018/S</t>
+  </si>
+  <si>
+    <t>PLD_4066/S</t>
+  </si>
+  <si>
+    <t>PLD_4107/S</t>
+  </si>
+  <si>
+    <t>PLD_4153</t>
+  </si>
+  <si>
+    <t>PLD_6012</t>
+  </si>
+  <si>
+    <t>PLD_6042_HAWANA</t>
+  </si>
+  <si>
+    <t>PLD_6042/S</t>
+  </si>
+  <si>
+    <t>PLD_6099/S</t>
+  </si>
+  <si>
+    <t>PLD_6175/S</t>
+  </si>
+  <si>
+    <t>PLD_6175/S_086</t>
+  </si>
+  <si>
+    <t>PLD_6192/S</t>
+  </si>
+  <si>
+    <t>PLD_6193/S</t>
+  </si>
+  <si>
+    <t>PLD_6206_KB7GREY</t>
+  </si>
+  <si>
+    <t>PLD_2160</t>
+  </si>
+  <si>
+    <t>PLD_4066_086_HAV</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Open Sans"/>
     </font>
   </fonts>
   <fills count="2">
@@ -492,13 +671,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF45818E"/>
+          <bgColor rgb="FF45818E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF45818E"/>
+          <bgColor rgb="FF45818E"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -774,18 +983,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D141"/>
+  <dimension ref="A1:D200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="21.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>140</v>
       </c>
@@ -799,7 +1008,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -813,7 +1022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -827,7 +1036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -841,7 +1050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -855,7 +1064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -869,7 +1078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -883,7 +1092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -897,7 +1106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -911,7 +1120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -925,7 +1134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -939,7 +1148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -953,7 +1162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -967,7 +1176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -981,7 +1190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -995,7 +1204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1009,7 +1218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1023,7 +1232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1037,7 +1246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1051,7 +1260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1065,7 +1274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1079,7 +1288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1093,7 +1302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1107,7 +1316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1121,7 +1330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1135,7 +1344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1149,7 +1358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1163,7 +1372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1177,7 +1386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1191,7 +1400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1205,7 +1414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1219,7 +1428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1233,7 +1442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1247,7 +1456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1261,7 +1470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1275,7 +1484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1289,7 +1498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1303,7 +1512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1317,7 +1526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1331,7 +1540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -1345,7 +1554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -1359,7 +1568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -1373,7 +1582,7 @@
         <v>3748</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -1387,7 +1596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -1401,7 +1610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -1415,7 +1624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -1429,7 +1638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -1443,7 +1652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -1457,7 +1666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -1471,7 +1680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -1485,7 +1694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -1499,7 +1708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -1513,7 +1722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -1527,7 +1736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -1541,7 +1750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -1555,7 +1764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -1569,7 +1778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -1583,7 +1792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -1597,7 +1806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -1611,7 +1820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -1625,7 +1834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -1639,7 +1848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -1653,7 +1862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -1667,7 +1876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -1681,7 +1890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4">
       <c r="A65" t="s">
         <v>63</v>
       </c>
@@ -1695,7 +1904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4">
       <c r="A66" t="s">
         <v>64</v>
       </c>
@@ -1709,7 +1918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4">
       <c r="A67" t="s">
         <v>65</v>
       </c>
@@ -1723,7 +1932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4">
       <c r="A68" t="s">
         <v>66</v>
       </c>
@@ -1737,7 +1946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4">
       <c r="A69" t="s">
         <v>67</v>
       </c>
@@ -1751,7 +1960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -1765,7 +1974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -1779,7 +1988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -1793,7 +2002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4">
       <c r="A73" t="s">
         <v>71</v>
       </c>
@@ -1807,7 +2016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4">
       <c r="A74" t="s">
         <v>72</v>
       </c>
@@ -1821,7 +2030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4">
       <c r="A75" t="s">
         <v>73</v>
       </c>
@@ -1835,7 +2044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4">
       <c r="A76" t="s">
         <v>74</v>
       </c>
@@ -1849,7 +2058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4">
       <c r="A77" t="s">
         <v>75</v>
       </c>
@@ -1863,7 +2072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4">
       <c r="A78" t="s">
         <v>76</v>
       </c>
@@ -1877,7 +2086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4">
       <c r="A79" t="s">
         <v>77</v>
       </c>
@@ -1891,7 +2100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4">
       <c r="A80" t="s">
         <v>78</v>
       </c>
@@ -1905,7 +2114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4">
       <c r="A81" t="s">
         <v>79</v>
       </c>
@@ -1919,7 +2128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4">
       <c r="A82" t="s">
         <v>80</v>
       </c>
@@ -1933,7 +2142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4">
       <c r="A83" t="s">
         <v>81</v>
       </c>
@@ -1947,7 +2156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4">
       <c r="A84" t="s">
         <v>82</v>
       </c>
@@ -1961,7 +2170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4">
       <c r="A85" t="s">
         <v>83</v>
       </c>
@@ -1975,7 +2184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4">
       <c r="A86" t="s">
         <v>84</v>
       </c>
@@ -1989,7 +2198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4">
       <c r="A87" t="s">
         <v>85</v>
       </c>
@@ -2003,7 +2212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4">
       <c r="A88" t="s">
         <v>86</v>
       </c>
@@ -2017,7 +2226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4">
       <c r="A89" t="s">
         <v>87</v>
       </c>
@@ -2031,7 +2240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4">
       <c r="A90" t="s">
         <v>88</v>
       </c>
@@ -2045,7 +2254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4">
       <c r="A91" t="s">
         <v>89</v>
       </c>
@@ -2059,7 +2268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4">
       <c r="A92" t="s">
         <v>90</v>
       </c>
@@ -2073,7 +2282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4">
       <c r="A93" t="s">
         <v>91</v>
       </c>
@@ -2087,7 +2296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4">
       <c r="A94" t="s">
         <v>92</v>
       </c>
@@ -2101,7 +2310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4">
       <c r="A95" t="s">
         <v>93</v>
       </c>
@@ -2115,7 +2324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4">
       <c r="A96" t="s">
         <v>94</v>
       </c>
@@ -2129,7 +2338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4">
       <c r="A97" t="s">
         <v>95</v>
       </c>
@@ -2143,7 +2352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4">
       <c r="A98" t="s">
         <v>96</v>
       </c>
@@ -2157,7 +2366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4">
       <c r="A99" t="s">
         <v>97</v>
       </c>
@@ -2171,7 +2380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4">
       <c r="A100" t="s">
         <v>98</v>
       </c>
@@ -2185,7 +2394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4">
       <c r="A101" t="s">
         <v>99</v>
       </c>
@@ -2199,7 +2408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4">
       <c r="A102" t="s">
         <v>100</v>
       </c>
@@ -2213,7 +2422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4">
       <c r="A103" t="s">
         <v>101</v>
       </c>
@@ -2227,7 +2436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4">
       <c r="A104" t="s">
         <v>102</v>
       </c>
@@ -2241,7 +2450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4">
       <c r="A105" t="s">
         <v>103</v>
       </c>
@@ -2255,7 +2464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4">
       <c r="A106" t="s">
         <v>104</v>
       </c>
@@ -2269,7 +2478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4">
       <c r="A107" t="s">
         <v>105</v>
       </c>
@@ -2283,7 +2492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4">
       <c r="A108" t="s">
         <v>106</v>
       </c>
@@ -2297,7 +2506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4">
       <c r="A109" t="s">
         <v>107</v>
       </c>
@@ -2311,7 +2520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4">
       <c r="A110" t="s">
         <v>108</v>
       </c>
@@ -2325,7 +2534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4">
       <c r="A111" t="s">
         <v>109</v>
       </c>
@@ -2339,7 +2548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4">
       <c r="A112" t="s">
         <v>110</v>
       </c>
@@ -2353,7 +2562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:4">
       <c r="A113" t="s">
         <v>111</v>
       </c>
@@ -2367,7 +2576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4">
       <c r="A114" t="s">
         <v>112</v>
       </c>
@@ -2381,7 +2590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4">
       <c r="A115" t="s">
         <v>113</v>
       </c>
@@ -2395,7 +2604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4">
       <c r="A116" t="s">
         <v>114</v>
       </c>
@@ -2409,7 +2618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4">
       <c r="A117" t="s">
         <v>115</v>
       </c>
@@ -2423,7 +2632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:4">
       <c r="A118" t="s">
         <v>116</v>
       </c>
@@ -2437,7 +2646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:4">
       <c r="A119" t="s">
         <v>117</v>
       </c>
@@ -2451,7 +2660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:4">
       <c r="A120" t="s">
         <v>118</v>
       </c>
@@ -2465,7 +2674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:4">
       <c r="A121" t="s">
         <v>119</v>
       </c>
@@ -2479,7 +2688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:4">
       <c r="A122" t="s">
         <v>120</v>
       </c>
@@ -2493,7 +2702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:4">
       <c r="A123" t="s">
         <v>121</v>
       </c>
@@ -2507,7 +2716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:4">
       <c r="A124" t="s">
         <v>122</v>
       </c>
@@ -2521,7 +2730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:4">
       <c r="A125" t="s">
         <v>123</v>
       </c>
@@ -2535,7 +2744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:4">
       <c r="A126" t="s">
         <v>124</v>
       </c>
@@ -2549,7 +2758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:4">
       <c r="A127" t="s">
         <v>125</v>
       </c>
@@ -2563,7 +2772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:4">
       <c r="A128" t="s">
         <v>126</v>
       </c>
@@ -2577,7 +2786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:4">
       <c r="A129" t="s">
         <v>127</v>
       </c>
@@ -2591,7 +2800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:4">
       <c r="A130" t="s">
         <v>128</v>
       </c>
@@ -2605,7 +2814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:4">
       <c r="A131" t="s">
         <v>129</v>
       </c>
@@ -2619,7 +2828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:4">
       <c r="A132" t="s">
         <v>130</v>
       </c>
@@ -2633,7 +2842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:4">
       <c r="A133" t="s">
         <v>131</v>
       </c>
@@ -2647,7 +2856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:4">
       <c r="A134" t="s">
         <v>132</v>
       </c>
@@ -2661,7 +2870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:4">
       <c r="A135" t="s">
         <v>133</v>
       </c>
@@ -2675,7 +2884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:4">
       <c r="A136" t="s">
         <v>134</v>
       </c>
@@ -2689,7 +2898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:4">
       <c r="A137" t="s">
         <v>135</v>
       </c>
@@ -2703,7 +2912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:4">
       <c r="A138" t="s">
         <v>136</v>
       </c>
@@ -2717,7 +2926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:4">
       <c r="A139" t="s">
         <v>137</v>
       </c>
@@ -2731,7 +2940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:4">
       <c r="A140" t="s">
         <v>138</v>
       </c>
@@ -2745,7 +2954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:4">
       <c r="A141" t="s">
         <v>139</v>
       </c>
@@ -2759,7 +2968,839 @@
         <v>0</v>
       </c>
     </row>
+    <row r="142" spans="1:4">
+      <c r="A142" t="s">
+        <v>144</v>
+      </c>
+      <c r="B142">
+        <v>0</v>
+      </c>
+      <c r="C142">
+        <v>825</v>
+      </c>
+      <c r="D142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
+      <c r="A143" t="s">
+        <v>145</v>
+      </c>
+      <c r="B143">
+        <v>0</v>
+      </c>
+      <c r="C143">
+        <v>10650</v>
+      </c>
+      <c r="D143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
+      <c r="A144" t="s">
+        <v>146</v>
+      </c>
+      <c r="B144">
+        <v>0</v>
+      </c>
+      <c r="C144">
+        <v>8695</v>
+      </c>
+      <c r="D144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
+      <c r="A145" t="s">
+        <v>147</v>
+      </c>
+      <c r="B145">
+        <v>0</v>
+      </c>
+      <c r="C145">
+        <v>2120</v>
+      </c>
+      <c r="D145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146" t="s">
+        <v>148</v>
+      </c>
+      <c r="B146">
+        <v>0</v>
+      </c>
+      <c r="C146">
+        <v>21446</v>
+      </c>
+      <c r="D146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
+      <c r="A147" t="s">
+        <v>149</v>
+      </c>
+      <c r="B147">
+        <v>15000</v>
+      </c>
+      <c r="C147">
+        <v>21010</v>
+      </c>
+      <c r="D147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
+      <c r="A148" t="s">
+        <v>150</v>
+      </c>
+      <c r="B148">
+        <v>0</v>
+      </c>
+      <c r="C148">
+        <v>4551</v>
+      </c>
+      <c r="D148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149" t="s">
+        <v>151</v>
+      </c>
+      <c r="B149">
+        <v>0</v>
+      </c>
+      <c r="C149">
+        <v>5700</v>
+      </c>
+      <c r="D149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
+      <c r="A150" t="s">
+        <v>152</v>
+      </c>
+      <c r="B150">
+        <v>0</v>
+      </c>
+      <c r="C150">
+        <v>1630</v>
+      </c>
+      <c r="D150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
+      <c r="A151" t="s">
+        <v>153</v>
+      </c>
+      <c r="B151">
+        <v>0</v>
+      </c>
+      <c r="C151">
+        <v>4681</v>
+      </c>
+      <c r="D151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4">
+      <c r="A152" t="s">
+        <v>154</v>
+      </c>
+      <c r="B152">
+        <v>0</v>
+      </c>
+      <c r="C152">
+        <v>4340</v>
+      </c>
+      <c r="D152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4">
+      <c r="A153" t="s">
+        <v>155</v>
+      </c>
+      <c r="B153">
+        <v>0</v>
+      </c>
+      <c r="C153">
+        <v>700</v>
+      </c>
+      <c r="D153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4">
+      <c r="A154" t="s">
+        <v>156</v>
+      </c>
+      <c r="B154">
+        <v>0</v>
+      </c>
+      <c r="C154">
+        <v>1000</v>
+      </c>
+      <c r="D154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4">
+      <c r="A155" t="s">
+        <v>157</v>
+      </c>
+      <c r="B155">
+        <v>0</v>
+      </c>
+      <c r="C155">
+        <v>5701</v>
+      </c>
+      <c r="D155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4">
+      <c r="A156" t="s">
+        <v>158</v>
+      </c>
+      <c r="B156">
+        <v>0</v>
+      </c>
+      <c r="C156">
+        <v>3900</v>
+      </c>
+      <c r="D156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4">
+      <c r="A157" t="s">
+        <v>159</v>
+      </c>
+      <c r="B157">
+        <v>0</v>
+      </c>
+      <c r="C157">
+        <v>0</v>
+      </c>
+      <c r="D157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4">
+      <c r="A158" t="s">
+        <v>160</v>
+      </c>
+      <c r="B158">
+        <v>0</v>
+      </c>
+      <c r="C158">
+        <v>18260</v>
+      </c>
+      <c r="D158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4">
+      <c r="A159" t="s">
+        <v>161</v>
+      </c>
+      <c r="B159">
+        <v>0</v>
+      </c>
+      <c r="C159">
+        <v>0</v>
+      </c>
+      <c r="D159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4">
+      <c r="A160" t="s">
+        <v>162</v>
+      </c>
+      <c r="B160">
+        <v>0</v>
+      </c>
+      <c r="C160">
+        <v>1700</v>
+      </c>
+      <c r="D160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4">
+      <c r="A161" t="s">
+        <v>163</v>
+      </c>
+      <c r="B161" s="2">
+        <v>0</v>
+      </c>
+      <c r="C161" s="2">
+        <v>2345</v>
+      </c>
+      <c r="D161" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4">
+      <c r="A162" s="1" t="str">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Бумага крепированная, неотбеленная, МЦБК")</f>
+        <v>Бумага крепированная, неотбеленная, МЦБК</v>
+      </c>
+      <c r="B162" s="3">
+        <v>0</v>
+      </c>
+      <c r="C162" s="3">
+        <v>695</v>
+      </c>
+      <c r="D162" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4">
+      <c r="A163" t="s">
+        <v>164</v>
+      </c>
+      <c r="B163" s="2">
+        <v>0</v>
+      </c>
+      <c r="C163" s="2">
+        <v>200</v>
+      </c>
+      <c r="D163" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4">
+      <c r="A164" t="s">
+        <v>165</v>
+      </c>
+      <c r="B164">
+        <v>1200</v>
+      </c>
+      <c r="C164">
+        <v>1400</v>
+      </c>
+      <c r="D164" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4">
+      <c r="A165" t="s">
+        <v>166</v>
+      </c>
+      <c r="B165">
+        <v>0</v>
+      </c>
+      <c r="C165">
+        <v>0</v>
+      </c>
+      <c r="D165" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4">
+      <c r="A166" t="s">
+        <v>167</v>
+      </c>
+      <c r="B166">
+        <v>0</v>
+      </c>
+      <c r="C166">
+        <v>450</v>
+      </c>
+      <c r="D166" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4">
+      <c r="A167" t="s">
+        <v>168</v>
+      </c>
+      <c r="B167">
+        <v>0</v>
+      </c>
+      <c r="C167">
+        <v>400</v>
+      </c>
+      <c r="D167" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4">
+      <c r="A168" t="s">
+        <v>169</v>
+      </c>
+      <c r="B168">
+        <v>150</v>
+      </c>
+      <c r="C168">
+        <v>0</v>
+      </c>
+      <c r="D168" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4">
+      <c r="A169" t="s">
+        <v>170</v>
+      </c>
+      <c r="B169">
+        <v>0</v>
+      </c>
+      <c r="C169">
+        <v>980</v>
+      </c>
+      <c r="D169" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4">
+      <c r="A170" t="s">
+        <v>171</v>
+      </c>
+      <c r="B170">
+        <v>0</v>
+      </c>
+      <c r="C170">
+        <v>0</v>
+      </c>
+      <c r="D170" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4">
+      <c r="A171" t="s">
+        <v>172</v>
+      </c>
+      <c r="B171">
+        <v>0</v>
+      </c>
+      <c r="C171">
+        <v>0</v>
+      </c>
+      <c r="D171">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4">
+      <c r="A172" t="s">
+        <v>173</v>
+      </c>
+      <c r="B172">
+        <v>0</v>
+      </c>
+      <c r="C172">
+        <v>0</v>
+      </c>
+      <c r="D172">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4">
+      <c r="A173" t="s">
+        <v>174</v>
+      </c>
+      <c r="B173">
+        <v>0</v>
+      </c>
+      <c r="C173">
+        <v>0</v>
+      </c>
+      <c r="D173">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4">
+      <c r="A174" t="s">
+        <v>175</v>
+      </c>
+      <c r="B174">
+        <v>0</v>
+      </c>
+      <c r="C174">
+        <v>0</v>
+      </c>
+      <c r="D174">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4">
+      <c r="A175" t="s">
+        <v>176</v>
+      </c>
+      <c r="B175">
+        <v>0</v>
+      </c>
+      <c r="C175">
+        <v>0</v>
+      </c>
+      <c r="D175">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4">
+      <c r="A176" t="s">
+        <v>177</v>
+      </c>
+      <c r="B176">
+        <v>0</v>
+      </c>
+      <c r="C176">
+        <v>0</v>
+      </c>
+      <c r="D176">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4">
+      <c r="A177" t="s">
+        <v>178</v>
+      </c>
+      <c r="B177">
+        <v>0</v>
+      </c>
+      <c r="C177">
+        <v>0</v>
+      </c>
+      <c r="D177">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4">
+      <c r="A178" t="s">
+        <v>179</v>
+      </c>
+      <c r="B178">
+        <v>0</v>
+      </c>
+      <c r="C178">
+        <v>0</v>
+      </c>
+      <c r="D178">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4">
+      <c r="A179" t="s">
+        <v>180</v>
+      </c>
+      <c r="B179">
+        <v>0</v>
+      </c>
+      <c r="C179">
+        <v>0</v>
+      </c>
+      <c r="D179">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4">
+      <c r="A180" t="s">
+        <v>181</v>
+      </c>
+      <c r="B180">
+        <v>0</v>
+      </c>
+      <c r="C180">
+        <v>0</v>
+      </c>
+      <c r="D180">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4">
+      <c r="A181" t="s">
+        <v>182</v>
+      </c>
+      <c r="B181">
+        <v>0</v>
+      </c>
+      <c r="C181">
+        <v>0</v>
+      </c>
+      <c r="D181">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4">
+      <c r="A182" t="s">
+        <v>183</v>
+      </c>
+      <c r="B182">
+        <v>0</v>
+      </c>
+      <c r="C182">
+        <v>0</v>
+      </c>
+      <c r="D182">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4">
+      <c r="A183" t="s">
+        <v>184</v>
+      </c>
+      <c r="B183">
+        <v>0</v>
+      </c>
+      <c r="C183">
+        <v>0</v>
+      </c>
+      <c r="D183">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4">
+      <c r="A184" t="s">
+        <v>185</v>
+      </c>
+      <c r="B184">
+        <v>0</v>
+      </c>
+      <c r="C184">
+        <v>0</v>
+      </c>
+      <c r="D184">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4">
+      <c r="A185" t="s">
+        <v>186</v>
+      </c>
+      <c r="B185">
+        <v>0</v>
+      </c>
+      <c r="C185">
+        <v>0</v>
+      </c>
+      <c r="D185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4">
+      <c r="A186" t="s">
+        <v>187</v>
+      </c>
+      <c r="B186">
+        <v>0</v>
+      </c>
+      <c r="C186">
+        <v>0</v>
+      </c>
+      <c r="D186">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4">
+      <c r="A187" t="s">
+        <v>188</v>
+      </c>
+      <c r="B187">
+        <v>0</v>
+      </c>
+      <c r="C187">
+        <v>0</v>
+      </c>
+      <c r="D187">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4">
+      <c r="A188" t="s">
+        <v>189</v>
+      </c>
+      <c r="B188">
+        <v>0</v>
+      </c>
+      <c r="C188">
+        <v>0</v>
+      </c>
+      <c r="D188">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4">
+      <c r="A189" t="s">
+        <v>190</v>
+      </c>
+      <c r="B189">
+        <v>0</v>
+      </c>
+      <c r="C189">
+        <v>0</v>
+      </c>
+      <c r="D189">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4">
+      <c r="A190" t="s">
+        <v>191</v>
+      </c>
+      <c r="B190">
+        <v>0</v>
+      </c>
+      <c r="C190">
+        <v>0</v>
+      </c>
+      <c r="D190">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4">
+      <c r="A191" t="s">
+        <v>192</v>
+      </c>
+      <c r="B191">
+        <v>0</v>
+      </c>
+      <c r="C191">
+        <v>0</v>
+      </c>
+      <c r="D191">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4">
+      <c r="A192" t="s">
+        <v>193</v>
+      </c>
+      <c r="B192">
+        <v>0</v>
+      </c>
+      <c r="C192">
+        <v>0</v>
+      </c>
+      <c r="D192">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4">
+      <c r="A193" t="s">
+        <v>194</v>
+      </c>
+      <c r="B193">
+        <v>0</v>
+      </c>
+      <c r="C193">
+        <v>0</v>
+      </c>
+      <c r="D193">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4">
+      <c r="A194" t="s">
+        <v>195</v>
+      </c>
+      <c r="B194">
+        <v>0</v>
+      </c>
+      <c r="C194">
+        <v>0</v>
+      </c>
+      <c r="D194">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4">
+      <c r="A195" t="s">
+        <v>196</v>
+      </c>
+      <c r="B195">
+        <v>0</v>
+      </c>
+      <c r="C195">
+        <v>0</v>
+      </c>
+      <c r="D195">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4">
+      <c r="A196" t="s">
+        <v>197</v>
+      </c>
+      <c r="B196">
+        <v>0</v>
+      </c>
+      <c r="C196">
+        <v>0</v>
+      </c>
+      <c r="D196">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4">
+      <c r="A197" t="s">
+        <v>198</v>
+      </c>
+      <c r="B197">
+        <v>0</v>
+      </c>
+      <c r="C197">
+        <v>0</v>
+      </c>
+      <c r="D197">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4">
+      <c r="A198" t="s">
+        <v>199</v>
+      </c>
+      <c r="B198">
+        <v>0</v>
+      </c>
+      <c r="C198">
+        <v>0</v>
+      </c>
+      <c r="D198">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4">
+      <c r="A199" t="s">
+        <v>200</v>
+      </c>
+      <c r="B199">
+        <v>0</v>
+      </c>
+      <c r="C199">
+        <v>0</v>
+      </c>
+      <c r="D199">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4">
+      <c r="A200" t="s">
+        <v>201</v>
+      </c>
+      <c r="B200">
+        <v>0</v>
+      </c>
+      <c r="C200">
+        <v>0</v>
+      </c>
+      <c r="D200">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="A162">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>$D162=1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>